<commit_message>
Editing Grade Sheet! (Only Works for sheet 15)
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,199 +445,194 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>440009</v>
+        <v>1180128</v>
       </c>
       <c r="B2" t="n">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>49</v>
-      </c>
-      <c r="B3" t="n">
+        <v>1190255</v>
+      </c>
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>4</v>
-      </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4490961</v>
+        <v>1180274</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>419097</v>
+        <v>1180056</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>6</v>
+        <v>1180041</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4904</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
+        <v>1180606</v>
       </c>
       <c r="C7" t="n">
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>449060</v>
+        <v>1180456</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>2200022</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>1180552</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>44</v>
+        <v>1180207</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>49000</v>
+        <v>1180045</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>790</v>
+        <v>1180212</v>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>44001</v>
+        <v>1180155</v>
+      </c>
+      <c r="B14" t="n">
+        <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>49</v>
+        <v>1470343</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>447024</v>
+        <v>1190172</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>4017</v>
-      </c>
-      <c r="C17" t="n">
-        <v>4</v>
-      </c>
-      <c r="D17" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>